<commit_message>
drop & cond checker
</commit_message>
<xml_diff>
--- a/plan/excel/drop_掉落表.xlsx
+++ b/plan/excel/drop_掉落表.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Break" sheetId="4" r:id="rId1"/>
+    <sheet name="Drop" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Break!$A$1:$B$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Drop!$A$1:$A$4</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -19,7 +19,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>作者</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="C1" authorId="0" shapeId="0">
@@ -33,7 +33,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>作者:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -44,7 +44,26 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-必定掉落的</t>
+每一项，都是</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>10000</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>分之的概率</t>
         </r>
       </text>
     </comment>
@@ -59,7 +78,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>作者:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -70,7 +89,59 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-适用于条件开启</t>
+权重之和为10000，不足则可能轮空(注：最多只可能掉落一项)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+条件ID满足时，执行概率掉落</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+条件表中配置的ID，为真时执行条件掉落项，0表示不执行</t>
         </r>
       </text>
     </comment>
@@ -79,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
   <si>
     <t>number</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -89,52 +160,15 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>jl</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>number</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>dropId</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>掉落类型</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>dropType</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>掉落ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>jl</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>f</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ixed</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>map#id_cnt</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -155,31 +189,86 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>条件掉落ID</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>条件掉落项</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>cond</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>101_2|201_3</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>100_1|200_3</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>number</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>固定掉落项</t>
+    <t>jl</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1000_100_1|2000_200_3</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1000_100_1|2000_200_4</t>
+  </si>
+  <si>
+    <t>1000_100_1|2000_200_5</t>
+  </si>
+  <si>
+    <t>1000_100_1|2000_200_6</t>
+  </si>
+  <si>
+    <t>1000_100_1|2000_200_7</t>
+  </si>
+  <si>
+    <t>1000_100_1|2000_200_8</t>
+  </si>
+  <si>
+    <t>1000_100_1|2000_200_9</t>
+  </si>
+  <si>
+    <t>1000_100_1|2000_200_10</t>
+  </si>
+  <si>
+    <t>1000_100_1|2000_200_11</t>
+  </si>
+  <si>
+    <t>1000_100_1|2000_200_12</t>
+  </si>
+  <si>
+    <t>概率掉落项</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>权重掉落项</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>map</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>prob#prob_id_cnt</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>weight#prob_id_cnt</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>map</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>cond#prob_id_cnt</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>说明</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>主线任务第一关掉落</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>条件ID</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -187,7 +276,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +326,20 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -258,15 +361,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -282,7 +388,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -568,44 +674,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="24.875" customWidth="1"/>
-    <col min="5" max="5" width="22.125" customWidth="1"/>
+    <col min="3" max="5" width="24.875" customWidth="1"/>
+    <col min="6" max="6" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
@@ -613,130 +720,228 @@
         <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>22</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+        <v>25</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+        <v>24</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>10001</v>
       </c>
-      <c r="B5">
-        <v>1</v>
+      <c r="B5" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>10002</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>10003</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>10004</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>10005</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>10006</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>10007</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>10008</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>10009</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>10010</v>
       </c>
-      <c r="B14">
-        <v>1</v>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on upgrade talnet & aptitude
</commit_message>
<xml_diff>
--- a/plan/excel/drop_掉落表.xlsx
+++ b/plan/excel/drop_掉落表.xlsx
@@ -19,7 +19,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>作者</author>
   </authors>
   <commentList>
     <comment ref="C1" authorId="0" shapeId="0">
@@ -33,7 +33,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>Author:</t>
+          <t>作者:</t>
         </r>
         <r>
           <rPr>
@@ -78,7 +78,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>Author:</t>
+          <t>作者:</t>
         </r>
         <r>
           <rPr>
@@ -104,7 +104,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>Author:</t>
+          <t>作者:</t>
         </r>
         <r>
           <rPr>
@@ -130,7 +130,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>Author:</t>
+          <t>作者:</t>
         </r>
         <r>
           <rPr>
@@ -179,7 +179,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -201,37 +201,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>1000_100_1|2000_200_3</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>1000_100_1|2000_200_4</t>
-  </si>
-  <si>
-    <t>1000_100_1|2000_200_5</t>
-  </si>
-  <si>
-    <t>1000_100_1|2000_200_6</t>
-  </si>
-  <si>
-    <t>1000_100_1|2000_200_7</t>
-  </si>
-  <si>
-    <t>1000_100_1|2000_200_8</t>
-  </si>
-  <si>
-    <t>1000_100_1|2000_200_9</t>
-  </si>
-  <si>
-    <t>1000_100_1|2000_200_10</t>
-  </si>
-  <si>
-    <t>1000_100_1|2000_200_11</t>
-  </si>
-  <si>
-    <t>1000_100_1|2000_200_12</t>
-  </si>
-  <si>
     <t>概率掉落项</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -270,17 +239,47 @@
   <si>
     <t>条件ID</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1000_4002_1|2000_4013_3</t>
+  </si>
+  <si>
+    <t>1000_4002_1|2000_4013_4</t>
+  </si>
+  <si>
+    <t>1000_4002_1|2000_4013_5</t>
+  </si>
+  <si>
+    <t>1000_4002_1|2000_4013_6</t>
+  </si>
+  <si>
+    <t>1000_4002_1|2000_4013_7</t>
+  </si>
+  <si>
+    <t>1000_4002_1|2000_4013_8</t>
+  </si>
+  <si>
+    <t>1000_4002_1|2000_4013_9</t>
+  </si>
+  <si>
+    <t>1000_4002_1|2000_4013_10</t>
+  </si>
+  <si>
+    <t>1000_4002_1|2000_4013_11</t>
+  </si>
+  <si>
+    <t>1000_4002_1|2000_4013_12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -299,14 +298,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -335,7 +334,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF333333"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -372,7 +371,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -388,7 +387,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -678,37 +677,39 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5:E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="24.875" customWidth="1"/>
-    <col min="6" max="6" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" customWidth="1"/>
+    <col min="4" max="4" width="36.42578125" customWidth="1"/>
+    <col min="5" max="5" width="35.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -726,219 +727,219 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>10001</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>10002</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>10003</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>10004</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>10005</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>10006</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>10007</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>10008</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="F12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>10009</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="F13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>10010</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="F14">
         <v>2</v>

</xml_diff>